<commit_message>
change in convenios data
</commit_message>
<xml_diff>
--- a/microservices/extract_convenios/data/raw/convenios.xlsx
+++ b/microservices/extract_convenios/data/raw/convenios.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apabook/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apabook/Public/esd-api/wp-content/themes/ESD_api/microservices/extract_convenios/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE472CC6-A107-934D-B185-56F3D6EF61C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B578AD60-1E57-324C-941D-CE09866157D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{6579D923-BC5F-174A-AB2D-CFFCED0F0EF1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="215">
   <si>
     <t>alemania</t>
   </si>
@@ -619,6 +619,57 @@
   </si>
   <si>
     <t>london</t>
+  </si>
+  <si>
+    <t>Sint-Lukas Hogeschool Voor Wetenschap &amp; Kunst</t>
+  </si>
+  <si>
+    <t>https://www.sintlucas.wenk.be/</t>
+  </si>
+  <si>
+    <t>españa</t>
+  </si>
+  <si>
+    <t>spain</t>
+  </si>
+  <si>
+    <t>madrid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Escuela Superior de Diseño de Madrid </t>
+  </si>
+  <si>
+    <t>https://esdmadrid.es</t>
+  </si>
+  <si>
+    <t>Universidad Complutense de Madrid - Facultad de Bellas Artes</t>
+  </si>
+  <si>
+    <t>https://www.bellasartes.ucm.es/</t>
+  </si>
+  <si>
+    <t>creta</t>
+  </si>
+  <si>
+    <t>crete</t>
+  </si>
+  <si>
+    <t>Technical University of Crete</t>
+  </si>
+  <si>
+    <t>https://en.tuc.gr/offline-en.html</t>
+  </si>
+  <si>
+    <t>Universidade do Porto - Faculdade de Belas Artes</t>
+  </si>
+  <si>
+    <t>https://sigarra.up.pt/fbaup/pt/web_page.inicial</t>
+  </si>
+  <si>
+    <t>University of the Arts London - Chelsea College of Art and Design</t>
+  </si>
+  <si>
+    <t>https://www.chelsea.arts.ac.uk/</t>
   </si>
 </sst>
 </file>
@@ -981,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25AF432D-0A23-F84B-B3CB-F1BD26336923}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="157" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -993,7 +1044,7 @@
     <col min="7" max="7" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>0</v>
       </c>
@@ -1018,8 +1069,14 @@
       <c r="H1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1044,8 +1101,14 @@
       <c r="H2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>167</v>
+      </c>
+      <c r="J2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1070,8 +1133,14 @@
       <c r="H3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>167</v>
+      </c>
+      <c r="J3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1096,8 +1165,14 @@
       <c r="H4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>167</v>
+      </c>
+      <c r="J4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1122,8 +1197,14 @@
       <c r="H5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>167</v>
+      </c>
+      <c r="J5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1148,8 +1229,14 @@
       <c r="H6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>167</v>
+      </c>
+      <c r="J6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1174,8 +1261,14 @@
       <c r="H7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>167</v>
+      </c>
+      <c r="J7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1200,8 +1293,14 @@
       <c r="H8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1226,8 +1325,14 @@
       <c r="H9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>167</v>
+      </c>
+      <c r="J9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1252,8 +1357,14 @@
       <c r="H10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>167</v>
+      </c>
+      <c r="J10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1278,8 +1389,14 @@
       <c r="H11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>167</v>
+      </c>
+      <c r="J11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1304,8 +1421,14 @@
       <c r="H12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>167</v>
+      </c>
+      <c r="J12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1330,8 +1453,14 @@
       <c r="H13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>167</v>
+      </c>
+      <c r="J13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1356,8 +1485,14 @@
       <c r="H14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>167</v>
+      </c>
+      <c r="J14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1382,8 +1517,14 @@
       <c r="H15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>167</v>
+      </c>
+      <c r="J15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1408,8 +1549,14 @@
       <c r="H16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" t="s">
+        <v>167</v>
+      </c>
+      <c r="J16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1434,8 +1581,14 @@
       <c r="H17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" t="s">
+        <v>167</v>
+      </c>
+      <c r="J17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1460,8 +1613,14 @@
       <c r="H18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>167</v>
+      </c>
+      <c r="J18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1486,8 +1645,14 @@
       <c r="H19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>167</v>
+      </c>
+      <c r="J19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1512,8 +1677,14 @@
       <c r="H20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" t="s">
+        <v>167</v>
+      </c>
+      <c r="J20" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1538,8 +1709,14 @@
       <c r="H21" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" t="s">
+        <v>167</v>
+      </c>
+      <c r="J21" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1564,8 +1741,14 @@
       <c r="H22" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" t="s">
+        <v>167</v>
+      </c>
+      <c r="J22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1590,8 +1773,14 @@
       <c r="H23" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" t="s">
+        <v>167</v>
+      </c>
+      <c r="J23" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1616,8 +1805,14 @@
       <c r="H24" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" t="s">
+        <v>167</v>
+      </c>
+      <c r="J24" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1642,8 +1837,14 @@
       <c r="H25" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" t="s">
+        <v>167</v>
+      </c>
+      <c r="J25" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1668,8 +1869,14 @@
       <c r="H26" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" t="s">
+        <v>167</v>
+      </c>
+      <c r="J26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1694,8 +1901,14 @@
       <c r="H27" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" t="s">
+        <v>167</v>
+      </c>
+      <c r="J27" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1720,8 +1933,14 @@
       <c r="H28" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" t="s">
+        <v>167</v>
+      </c>
+      <c r="J28" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1746,8 +1965,14 @@
       <c r="H29" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" t="s">
+        <v>167</v>
+      </c>
+      <c r="J29" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1772,8 +1997,14 @@
       <c r="H30" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" t="s">
+        <v>167</v>
+      </c>
+      <c r="J30" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1798,8 +2029,14 @@
       <c r="H31" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31" t="s">
+        <v>167</v>
+      </c>
+      <c r="J31" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1824,8 +2061,14 @@
       <c r="H32" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32" t="s">
+        <v>167</v>
+      </c>
+      <c r="J32" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1850,8 +2093,14 @@
       <c r="H33" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33" t="s">
+        <v>167</v>
+      </c>
+      <c r="J33" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1876,8 +2125,14 @@
       <c r="H34" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34" t="s">
+        <v>167</v>
+      </c>
+      <c r="J34" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1902,8 +2157,14 @@
       <c r="H35" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35" t="s">
+        <v>167</v>
+      </c>
+      <c r="J35" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1928,8 +2189,14 @@
       <c r="H36" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36" t="s">
+        <v>167</v>
+      </c>
+      <c r="J36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1954,8 +2221,14 @@
       <c r="H37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37" t="s">
+        <v>167</v>
+      </c>
+      <c r="J37" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1980,8 +2253,14 @@
       <c r="H38" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38" t="s">
+        <v>167</v>
+      </c>
+      <c r="J38" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2006,8 +2285,14 @@
       <c r="H39" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I39" t="s">
+        <v>167</v>
+      </c>
+      <c r="J39" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2032,8 +2317,14 @@
       <c r="H40" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40" t="s">
+        <v>167</v>
+      </c>
+      <c r="J40" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2058,8 +2349,14 @@
       <c r="H41" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I41" t="s">
+        <v>36</v>
+      </c>
+      <c r="J41" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2084,8 +2381,14 @@
       <c r="H42" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I42" t="s">
+        <v>36</v>
+      </c>
+      <c r="J42" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2110,8 +2413,14 @@
       <c r="H43" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I43" t="s">
+        <v>36</v>
+      </c>
+      <c r="J43" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2136,8 +2445,14 @@
       <c r="H44" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I44" t="s">
+        <v>36</v>
+      </c>
+      <c r="J44" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2162,8 +2477,14 @@
       <c r="H45" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I45" t="s">
+        <v>36</v>
+      </c>
+      <c r="J45" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2188,8 +2509,14 @@
       <c r="H46" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I46" t="s">
+        <v>36</v>
+      </c>
+      <c r="J46" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2214,8 +2541,14 @@
       <c r="H47" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I47" t="s">
+        <v>36</v>
+      </c>
+      <c r="J47" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2239,6 +2572,204 @@
       </c>
       <c r="H48" t="s">
         <v>167</v>
+      </c>
+      <c r="I48" t="s">
+        <v>36</v>
+      </c>
+      <c r="J48" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" t="s">
+        <v>40</v>
+      </c>
+      <c r="E49" t="s">
+        <v>177</v>
+      </c>
+      <c r="F49" t="s">
+        <v>198</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H49" t="s">
+        <v>167</v>
+      </c>
+      <c r="I49" t="s">
+        <v>167</v>
+      </c>
+      <c r="J49" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>200</v>
+      </c>
+      <c r="C50" t="s">
+        <v>201</v>
+      </c>
+      <c r="D50" t="s">
+        <v>202</v>
+      </c>
+      <c r="E50" t="s">
+        <v>202</v>
+      </c>
+      <c r="F50" t="s">
+        <v>203</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H50" t="s">
+        <v>167</v>
+      </c>
+      <c r="I50" t="s">
+        <v>167</v>
+      </c>
+      <c r="J50" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>200</v>
+      </c>
+      <c r="C51" t="s">
+        <v>201</v>
+      </c>
+      <c r="D51" t="s">
+        <v>202</v>
+      </c>
+      <c r="E51" t="s">
+        <v>202</v>
+      </c>
+      <c r="F51" t="s">
+        <v>205</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H51" t="s">
+        <v>167</v>
+      </c>
+      <c r="I51" t="s">
+        <v>167</v>
+      </c>
+      <c r="J51" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" t="s">
+        <v>207</v>
+      </c>
+      <c r="E52" t="s">
+        <v>208</v>
+      </c>
+      <c r="F52" t="s">
+        <v>209</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H52" t="s">
+        <v>167</v>
+      </c>
+      <c r="I52" t="s">
+        <v>167</v>
+      </c>
+      <c r="J52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53" t="s">
+        <v>192</v>
+      </c>
+      <c r="F53" t="s">
+        <v>211</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="H53" t="s">
+        <v>167</v>
+      </c>
+      <c r="I53" t="s">
+        <v>167</v>
+      </c>
+      <c r="J53" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54" t="s">
+        <v>150</v>
+      </c>
+      <c r="E54" t="s">
+        <v>197</v>
+      </c>
+      <c r="F54" t="s">
+        <v>213</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H54" t="s">
+        <v>167</v>
+      </c>
+      <c r="I54" t="s">
+        <v>167</v>
+      </c>
+      <c r="J54" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2291,6 +2822,12 @@
     <hyperlink ref="G46" r:id="rId46" xr:uid="{31FF6F2D-542E-B347-B33E-112916194D8C}"/>
     <hyperlink ref="G47" r:id="rId47" xr:uid="{4B45ABEE-06F9-9A4F-847D-152C1F77C93B}"/>
     <hyperlink ref="G48" r:id="rId48" xr:uid="{A82B6028-4C4F-2E44-8C3A-56EA77087E21}"/>
+    <hyperlink ref="G49" r:id="rId49" xr:uid="{F05C0557-A10D-204B-AA91-D4614E1B9A23}"/>
+    <hyperlink ref="G50" r:id="rId50" xr:uid="{3D5C3A31-4D7D-C247-B2EC-2FBEDB2AE2E1}"/>
+    <hyperlink ref="G51" r:id="rId51" xr:uid="{87F6FE43-7E7B-CF46-B9EE-BDD77AE77A7E}"/>
+    <hyperlink ref="G52" r:id="rId52" xr:uid="{CC78964B-D4CE-7744-A9DD-95942B5F96E3}"/>
+    <hyperlink ref="G53" r:id="rId53" xr:uid="{22637000-40B9-0547-B1B4-BE719D11CA73}"/>
+    <hyperlink ref="G54" r:id="rId54" xr:uid="{BC8B7F9A-3E16-2143-A028-B3E54646A681}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>